<commit_message>
add campos de tablas db
</commit_message>
<xml_diff>
--- a/clases en uml.xlsx
+++ b/clases en uml.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abelthf/projects/login/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2C97437-29AB-D54A-BAA5-42A0A389E69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DEF2BE-4725-344F-BA68-A00B57ECFC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="1860" windowWidth="51200" windowHeight="21600" xr2:uid="{F72B4B69-7526-0B44-8808-4949CF77EB84}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Clases</t>
   </si>
@@ -52,13 +52,90 @@
 = recha_registro()
 = licenciaaprobada()</t>
   </si>
+  <si>
+    <t>Base de datos</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>empleado</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>- empleado_id</t>
+  </si>
+  <si>
+    <t>- licencia_enfermerdad</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>- licencia_maternidad</t>
+  </si>
+  <si>
+    <t>- licencia_emergencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -licencia_id</t>
+  </si>
+  <si>
+    <t>-licencia</t>
+  </si>
+  <si>
+    <t>- fecha_actual</t>
+  </si>
+  <si>
+    <t>- dias</t>
+  </si>
+  <si>
+    <t>- fecha1</t>
+  </si>
+  <si>
+    <t>- estado</t>
+  </si>
+  <si>
+    <t>- hrs_estado</t>
+  </si>
+  <si>
+    <t>- registro_id</t>
+  </si>
+  <si>
+    <t>- nombres</t>
+  </si>
+  <si>
+    <t>- numero_contacto</t>
+  </si>
+  <si>
+    <t>- emplado_mail</t>
+  </si>
+  <si>
+    <t>-empleado_direccion</t>
+  </si>
+  <si>
+    <t>- password</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,12 +178,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075B5D12-17E7-5943-AFB3-22F99FE38C24}">
-  <dimension ref="G4:O8"/>
+  <dimension ref="G4:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="270" zoomScaleNormal="270" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="270" zoomScaleNormal="270" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,6 +558,181 @@
       <c r="M8" s="1"/>
       <c r="O8" s="1"/>
     </row>
+    <row r="11" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="G11" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="G13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="G14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="G15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="G16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G19" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G29" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G35" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>